<commit_message>
Architecture implementation:    Avec deux ADCs du EGSE.    Avec piloatge carte Dispatch 8 ADCs.
Nouveau Pin_allocation_EGSE.xlsx pour utilisation deux sortie arbre d'horloge.

vue implementation
   Physiquement 9 ADCLTC2311_Driver.vhd
   10 SDO
   5 conv
   5 sclk
</commit_message>
<xml_diff>
--- a/PCB/Pin_allocation_EGSE.xlsx
+++ b/PCB/Pin_allocation_EGSE.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADC_ACQ_lvds_dispatch_check_out\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\07- MGSE - EGSE\03_EGSE\EGSE_Dispatch_Opal_Kelly\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DFCE9A-9DB7-4637-870C-B5556C78765E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11220" xr2:uid="{27EE1022-09C5-48A1-BDFA-C44C5179B2B3}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN_EGSE_Dispatch_Opal_Kelly_V5" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t>DU1</t>
   </si>
@@ -300,13 +301,82 @@
   </si>
   <si>
     <t>MC1_18_B34_L21N</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>ADC_CNV</t>
+  </si>
+  <si>
+    <t>MC1_60_B34_L8_P</t>
+  </si>
+  <si>
+    <t>AB3</t>
+  </si>
+  <si>
+    <t>ADC_SCK_P</t>
+  </si>
+  <si>
+    <t>ADC_SCK_N</t>
+  </si>
+  <si>
+    <t>MC1_38_B34_L11_P</t>
+  </si>
+  <si>
+    <t>MC1_40_B34_L11_N</t>
+  </si>
+  <si>
+    <t>ADC_SDO_FRONT_P</t>
+  </si>
+  <si>
+    <t>ADC_SDO_FRONT_N</t>
+  </si>
+  <si>
+    <t>MC1_46_B34_L22_P</t>
+  </si>
+  <si>
+    <t>MC1_48_B34_L22_N</t>
+  </si>
+  <si>
+    <t>AB8</t>
+  </si>
+  <si>
+    <t>AA8</t>
+  </si>
+  <si>
+    <t>ADC_SDO_BACK_P</t>
+  </si>
+  <si>
+    <t>ADC_SDO_BACK_N</t>
+  </si>
+  <si>
+    <t>MC1_50_B34_L6_P</t>
+  </si>
+  <si>
+    <t>MC1_52_B34_L6_N</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>Y4</t>
+  </si>
+  <si>
+    <t>AA4</t>
+  </si>
+  <si>
+    <t>PIN ALLOCATION EGSE DISPATCH/OPAL_KELLY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +390,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +434,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -446,18 +534,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,46 +606,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,54 +986,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FA4118-1DAE-43E5-B416-1A7DF69ACAD3}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:9" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2">
@@ -895,8 +1048,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -909,8 +1062,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:9" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -923,8 +1076,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:9" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2">
@@ -936,10 +1089,10 @@
       <c r="D7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2">
@@ -952,8 +1105,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:9" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
@@ -966,8 +1119,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2">
@@ -980,43 +1133,43 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>35</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1030,7 +1183,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1044,7 +1197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1225,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1239,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1100,15 +1253,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -1130,15 +1283,15 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1146,15 +1299,15 @@
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1168,7 +1321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1182,7 +1335,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1190,15 +1343,15 @@
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="F26" s="26"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1206,23 +1359,23 @@
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="F27" s="5"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
+    <row r="28" spans="1:7" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1389,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1403,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -1264,7 +1417,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -1278,7 +1431,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -1292,7 +1445,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -1306,7 +1459,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
@@ -1320,13 +1473,102 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+    <row r="36" spans="1:4" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="29"/>
+      <c r="C37" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="30"/>
+      <c r="C41" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="30"/>
+      <c r="C42" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="B37:B43"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A11:D11"/>

</xml_diff>